<commit_message>
updated the db model to contain a better table for countries and new tables for funding and keyword info
</commit_message>
<xml_diff>
--- a/map_to_db.xlsx
+++ b/map_to_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmsoltani\Downloads\Git\elsametric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67CCDBB1-839E-4590-AC91-21F546E49AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8634EB6-9084-4EDD-9AD3-97B347E96AF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{E4BE737B-DB12-4CF6-85CE-7113E9D4262C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="149">
   <si>
     <t>Field</t>
   </si>
@@ -483,7 +483,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,25 +491,13 @@
       <family val="2"/>
       <charset val="178"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="178"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -521,17 +509,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -582,7 +567,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E9EC2FD-1B85-4F44-9963-0674FF454F3A}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E9EC2FD-1B85-4F44-9963-0674FF454F3A}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I50" xr:uid="{9247DB64-E7B8-46FC-B3C7-BB0E49625A1A}">
     <filterColumn colId="3">
       <filters>
@@ -591,15 +576,15 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="7" xr3:uid="{C3AD55F7-A2AE-4D35-ABF6-2FAD0F2BC98C}" name="No." dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{2899C5DE-A789-4534-BF24-A33A4201BDA2}" name="Field" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{4EF6C49A-4139-45D2-8E27-BD1924F51D9F}" name="Sub Field" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{C3AD55F7-A2AE-4D35-ABF6-2FAD0F2BC98C}" name="No." dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{2899C5DE-A789-4534-BF24-A33A4201BDA2}" name="Field" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4EF6C49A-4139-45D2-8E27-BD1924F51D9F}" name="Sub Field" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{E0058E61-8D3F-440F-9AEE-57BA6ABD2D7C}" name="Include" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{57DF9892-08AF-4A55-B253-DC3F1B9A4FF2}" name="Scopus Type" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{9F4DD2F7-D8BD-4462-ACCF-80CCB597F3C8}" name="DB Type" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{FA2515F0-5F2D-45EE-851A-CA4AB75F7B70}" name="Table" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{D664EA55-1BA5-4664-80E6-AA115E1B70B6}" name="Column" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{CF00D252-1EBC-4673-B94A-D2726F93614A}" name="Description" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{57DF9892-08AF-4A55-B253-DC3F1B9A4FF2}" name="Scopus Type" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{9F4DD2F7-D8BD-4462-ACCF-80CCB597F3C8}" name="DB Type" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FA2515F0-5F2D-45EE-851A-CA4AB75F7B70}" name="Table" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D664EA55-1BA5-4664-80E6-AA115E1B70B6}" name="Column" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CF00D252-1EBC-4673-B94A-D2726F93614A}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D39A3F-ABF1-4E57-BF8D-15BA212A8C58}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,85 +1231,85 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>128</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="C15"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="C16"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1645,31 +1630,31 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>137</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1947,29 +1932,29 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="C44"/>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" t="s">
         <v>136</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" t="s">
         <v>117</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" t="s">
         <v>116</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2000,79 +1985,79 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="C46"/>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46" t="s">
         <v>137</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2" t="s">
+      <c r="G46"/>
+      <c r="H46" t="s">
         <v>127</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="C47"/>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" t="s">
         <v>137</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" t="s">
         <v>90</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" t="s">
         <v>126</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="C48"/>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" t="s">
         <v>136</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2" t="s">
+      <c r="G48"/>
+      <c r="H48" t="s">
         <v>125</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on some functions to turn scopus data into the database
</commit_message>
<xml_diff>
--- a/map_to_db.xlsx
+++ b/map_to_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmsoltani\Downloads\Git\elsametric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8634EB6-9084-4EDD-9AD3-97B347E96AF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE488F2-E69C-4590-B273-F3D22F824450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{E4BE737B-DB12-4CF6-85CE-7113E9D4262C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="149">
   <si>
     <t>Field</t>
   </si>
@@ -575,6 +575,9 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A3:I50">
+    <sortCondition ref="G1:G50"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="7" xr3:uid="{C3AD55F7-A2AE-4D35-ABF6-2FAD0F2BC98C}" name="No." dataDxfId="8"/>
     <tableColumn id="1" xr3:uid="{2899C5DE-A789-4534-BF24-A33A4201BDA2}" name="Field" dataDxfId="7"/>
@@ -889,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D39A3F-ABF1-4E57-BF8D-15BA212A8C58}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,13 +961,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
@@ -973,16 +976,16 @@
         <v>129</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1024,301 +1027,311 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" t="s">
         <v>137</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>78</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G14" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" t="s">
-        <v>120</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="b">
         <v>1</v>
@@ -1327,24 +1340,24 @@
         <v>131</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="b">
         <v>1</v>
@@ -1359,44 +1372,44 @@
         <v>90</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D19" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="b">
         <v>1</v>
@@ -1405,16 +1418,16 @@
         <v>131</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1436,10 +1449,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="b">
         <v>1</v>
@@ -1448,16 +1461,16 @@
         <v>131</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1530,28 +1543,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1573,118 +1586,106 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D30" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" t="s">
-        <v>94</v>
-      </c>
-      <c r="H31" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" t="s">
-        <v>52</v>
+      <c r="A31" s="1">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1749,31 +1750,28 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1811,81 +1809,83 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="A39">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39"/>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
         <v>137</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>112</v>
+      <c r="G39" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>114</v>
+      <c r="A41">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -1907,10 +1907,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D43" s="1" t="b">
         <v>1</v>
@@ -1919,77 +1919,79 @@
         <v>131</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44"/>
-      <c r="D44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" t="s">
-        <v>136</v>
-      </c>
-      <c r="G44" t="s">
-        <v>117</v>
-      </c>
-      <c r="H44" t="s">
-        <v>116</v>
-      </c>
-      <c r="I44" t="s">
-        <v>68</v>
+      <c r="A44" s="1">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>70</v>
+      <c r="A45">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" t="s">
+        <v>103</v>
+      </c>
+      <c r="I45" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C46"/>
       <c r="D46" t="b">
@@ -1999,22 +2001,24 @@
         <v>131</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
-      </c>
-      <c r="G46"/>
+        <v>143</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
       <c r="H46" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="I46" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="C47"/>
       <c r="D47" t="b">
@@ -2024,90 +2028,89 @@
         <v>131</v>
       </c>
       <c r="F47" t="s">
+        <v>143</v>
+      </c>
+      <c r="G47" t="s">
+        <v>91</v>
+      </c>
+      <c r="H47" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>49</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49"/>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" t="s">
         <v>137</v>
       </c>
-      <c r="G47" t="s">
-        <v>90</v>
-      </c>
-      <c r="H47" t="s">
-        <v>126</v>
-      </c>
-      <c r="I47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="G49"/>
+      <c r="H49" t="s">
+        <v>127</v>
+      </c>
+      <c r="I49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>75</v>
       </c>
-      <c r="C48"/>
-      <c r="D48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>131</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="C50"/>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" t="s">
         <v>136</v>
       </c>
-      <c r="G48"/>
-      <c r="H48" t="s">
+      <c r="G50"/>
+      <c r="H50" t="s">
         <v>125</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I50" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>